<commit_message>
addition to collation 6-24-13
</commit_message>
<xml_diff>
--- a/xml/Collation_MC-HR.13.xlsx
+++ b/xml/Collation_MC-HR.13.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
   <si>
     <t>MC</t>
   </si>
@@ -407,6 +407,60 @@
   </si>
   <si>
     <t>Philippe</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>king,</t>
+  </si>
+  <si>
+    <t>[161]</t>
+  </si>
+  <si>
+    <t>[line break indentations are short, c. 2 characters]</t>
+  </si>
+  <si>
+    <t>[line break indentations are long, c. 4 characters]</t>
+  </si>
+  <si>
+    <t>[161-165]</t>
+  </si>
+  <si>
+    <t>[entire poem seems to be printed in a significantly smaller font]</t>
+  </si>
+  <si>
+    <t>sin worth sinning</t>
+  </si>
+  <si>
+    <t>thing worth sinning</t>
+  </si>
+  <si>
+    <t>sorrows</t>
+  </si>
+  <si>
+    <t>sorrows,</t>
+  </si>
+  <si>
+    <t>shaken</t>
+  </si>
+  <si>
+    <t>skaken</t>
+  </si>
+  <si>
+    <t>flameless,</t>
+  </si>
+  <si>
+    <t>flameless;</t>
+  </si>
+  <si>
+    <t>[209]</t>
+  </si>
+  <si>
+    <t>[decorative --o-- b/w title and body of poem]</t>
+  </si>
+  <si>
+    <t>[no decoration between title and body of poem]</t>
   </si>
 </sst>
 </file>
@@ -420,7 +474,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -452,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -467,6 +527,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,8 +838,8 @@
   <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1128,52 +1194,114 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>159.11000000000001</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>175.9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>179.17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>187.7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>189.3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
@@ -1527,6 +1655,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A34:C35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed commented statements after <heads>; finished recto collation of MC13
</commit_message>
<xml_diff>
--- a/xml/Collation_MC-HR.13.xlsx
+++ b/xml/Collation_MC-HR.13.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="172">
   <si>
     <t>MC</t>
   </si>
@@ -461,6 +461,75 @@
   </si>
   <si>
     <t>[no decoration between title and body of poem]</t>
+  </si>
+  <si>
+    <t>223.20.</t>
+  </si>
+  <si>
+    <t>225.19.</t>
+  </si>
+  <si>
+    <t>229.5.</t>
+  </si>
+  <si>
+    <t>Goodnight, goodbye.</t>
+  </si>
+  <si>
+    <t>Good-night, good-bye.</t>
+  </si>
+  <si>
+    <t>243.24.</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t>beneath</t>
+  </si>
+  <si>
+    <t>251.f.</t>
+  </si>
+  <si>
+    <t>[footnote centered]</t>
+  </si>
+  <si>
+    <t>[footnote justified left]</t>
+  </si>
+  <si>
+    <t>257.20.</t>
+  </si>
+  <si>
+    <t>mine, I</t>
+  </si>
+  <si>
+    <t>mine I</t>
+  </si>
+  <si>
+    <t>Love's</t>
+  </si>
+  <si>
+    <t>love's</t>
+  </si>
+  <si>
+    <t>277.26.</t>
+  </si>
+  <si>
+    <t>295.10.</t>
+  </si>
+  <si>
+    <t>this;</t>
+  </si>
+  <si>
+    <t>this,</t>
+  </si>
+  <si>
+    <t>297.7.</t>
+  </si>
+  <si>
+    <t>autumn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autumn </t>
   </si>
 </sst>
 </file>
@@ -474,7 +543,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +568,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -512,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -532,6 +607,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -838,8 +919,8 @@
   <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="4" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1281,75 +1362,147 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
+      <c r="A45" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>